<commit_message>
Apriori algorithm applied to the new data and some changes were made to the code
</commit_message>
<xml_diff>
--- a/Apriori/AprioriProject-Excel/support_listesi.xlsx
+++ b/Apriori/AprioriProject-Excel/support_listesi.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edanu\Desktop\AprioriProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edanu\Desktop\Bitirme Projesi\AprioriProject-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23727563-0D51-411F-B508-7D0AEAF41D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC7373C-22E9-4C9D-87E3-00EDC290ED72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="492" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="293">
   <si>
     <t>Ürün</t>
   </si>
@@ -50,853 +37,868 @@
     <t>sut</t>
   </si>
   <si>
+    <t>gofret</t>
+  </si>
+  <si>
+    <t>ekmek</t>
+  </si>
+  <si>
     <t>biskuvi</t>
   </si>
   <si>
     <t>kek</t>
   </si>
   <si>
-    <t>gofret</t>
-  </si>
-  <si>
-    <t>ekmek</t>
+    <t>peynir</t>
   </si>
   <si>
     <t>su</t>
   </si>
   <si>
+    <t>tavuk</t>
+  </si>
+  <si>
+    <t>yogurt</t>
+  </si>
+  <si>
     <t>makarna</t>
   </si>
   <si>
-    <t>peynir</t>
-  </si>
-  <si>
-    <t>yogurt</t>
-  </si>
-  <si>
-    <t>tavuk</t>
-  </si>
-  <si>
     <t>gazli icecek</t>
   </si>
   <si>
     <t>cips</t>
   </si>
   <si>
+    <t>sakiz</t>
+  </si>
+  <si>
     <t>kahve</t>
   </si>
   <si>
+    <t>kraker</t>
+  </si>
+  <si>
     <t>yumurta</t>
   </si>
   <si>
-    <t>sakiz</t>
+    <t>patates</t>
   </si>
   <si>
     <t>ayran</t>
   </si>
   <si>
-    <t>kraker</t>
+    <t>meyve suyu</t>
   </si>
   <si>
     <t>domates</t>
   </si>
   <si>
-    <t>patates</t>
-  </si>
-  <si>
     <t>soguk cay</t>
   </si>
   <si>
+    <t>tatli</t>
+  </si>
+  <si>
+    <t>maden suyu</t>
+  </si>
+  <si>
+    <t>islak mendil</t>
+  </si>
+  <si>
+    <t>misir</t>
+  </si>
+  <si>
+    <t>elma</t>
+  </si>
+  <si>
     <t>tutun mamulu</t>
   </si>
   <si>
-    <t>tatli</t>
+    <t>dondurma</t>
+  </si>
+  <si>
+    <t>salatalik</t>
   </si>
   <si>
     <t>cekirdek</t>
   </si>
   <si>
-    <t>islak mendil</t>
+    <t>margarin</t>
   </si>
   <si>
     <t>sivi deterjan</t>
   </si>
   <si>
+    <t>pirinc</t>
+  </si>
+  <si>
+    <t>seker</t>
+  </si>
+  <si>
+    <t>limon</t>
+  </si>
+  <si>
     <t>kagit havlu</t>
   </si>
   <si>
-    <t>pirinc</t>
-  </si>
-  <si>
-    <t>salatalik</t>
-  </si>
-  <si>
-    <t>limon</t>
-  </si>
-  <si>
-    <t>maden suyu</t>
-  </si>
-  <si>
-    <t>elma</t>
-  </si>
-  <si>
-    <t>misir</t>
-  </si>
-  <si>
-    <t>meyve suyu</t>
+    <t>aycicek yagi</t>
+  </si>
+  <si>
+    <t>dondurulmus gida</t>
+  </si>
+  <si>
+    <t>muz</t>
+  </si>
+  <si>
+    <t>krema</t>
+  </si>
+  <si>
+    <t>jelibon</t>
+  </si>
+  <si>
+    <t>cerez</t>
+  </si>
+  <si>
+    <t>salca</t>
+  </si>
+  <si>
+    <t>siyah cay</t>
   </si>
   <si>
     <t>hazir kahve</t>
   </si>
   <si>
-    <t>salca</t>
-  </si>
-  <si>
     <t>arpa sehriye</t>
   </si>
   <si>
-    <t>aycicek yagi</t>
-  </si>
-  <si>
-    <t>margarin</t>
-  </si>
-  <si>
-    <t>seker</t>
-  </si>
-  <si>
-    <t>dondurma</t>
+    <t>un</t>
+  </si>
+  <si>
+    <t>bardak</t>
+  </si>
+  <si>
+    <t>kurabiye</t>
   </si>
   <si>
     <t>zeytin</t>
   </si>
   <si>
-    <t>muz</t>
-  </si>
-  <si>
-    <t>un</t>
+    <t>manti</t>
+  </si>
+  <si>
+    <t>findik krema</t>
+  </si>
+  <si>
+    <t>yufka</t>
+  </si>
+  <si>
+    <t>tuz</t>
+  </si>
+  <si>
+    <t>kofte</t>
+  </si>
+  <si>
+    <t>ped</t>
   </si>
   <si>
     <t>camasir suyu</t>
   </si>
   <si>
-    <t>jelibon</t>
-  </si>
-  <si>
-    <t>ped</t>
-  </si>
-  <si>
-    <t>siyah cay</t>
+    <t>mutfak seker</t>
+  </si>
+  <si>
+    <t>seftali</t>
+  </si>
+  <si>
+    <t>salam</t>
+  </si>
+  <si>
+    <t>limonata</t>
   </si>
   <si>
     <t>sogan</t>
   </si>
   <si>
-    <t>seftali</t>
-  </si>
-  <si>
     <t>sosis</t>
   </si>
   <si>
-    <t>krema</t>
-  </si>
-  <si>
     <t>tuvalet kagidi</t>
   </si>
   <si>
-    <t>kasar</t>
-  </si>
-  <si>
-    <t>yufka</t>
-  </si>
-  <si>
-    <t>kurabiye</t>
-  </si>
-  <si>
-    <t>findik krema</t>
-  </si>
-  <si>
-    <t>kofte</t>
+    <t>sampuan</t>
+  </si>
+  <si>
+    <t>biber</t>
+  </si>
+  <si>
+    <t>sabun</t>
+  </si>
+  <si>
+    <t>bulasik deterjan</t>
+  </si>
+  <si>
+    <t>pecete</t>
+  </si>
+  <si>
+    <t>et</t>
+  </si>
+  <si>
+    <t>irmik</t>
   </si>
   <si>
     <t>kaymak</t>
   </si>
   <si>
-    <t>dondurulmus gida</t>
-  </si>
-  <si>
-    <t>tuz</t>
-  </si>
-  <si>
-    <t>biber</t>
+    <t>serbet</t>
+  </si>
+  <si>
+    <t>tursu</t>
+  </si>
+  <si>
+    <t>kefir</t>
   </si>
   <si>
     <t>badem</t>
   </si>
   <si>
-    <t>salam</t>
-  </si>
-  <si>
-    <t>irmik</t>
-  </si>
-  <si>
-    <t>pecete</t>
-  </si>
-  <si>
-    <t>mutfak seker</t>
-  </si>
-  <si>
-    <t>bulasik deterjan</t>
-  </si>
-  <si>
-    <t>manti</t>
-  </si>
-  <si>
-    <t>kefir</t>
+    <t>sandvic</t>
   </si>
   <si>
     <t>pil</t>
   </si>
   <si>
+    <t>cilt bakim</t>
+  </si>
+  <si>
+    <t>nutella</t>
+  </si>
+  <si>
+    <t>meyveli yogurt</t>
+  </si>
+  <si>
+    <t>mantar</t>
+  </si>
+  <si>
     <t>pul biber</t>
   </si>
   <si>
-    <t>sampuan</t>
-  </si>
-  <si>
-    <t>et</t>
+    <t>tereyag</t>
+  </si>
+  <si>
+    <t>yer fistigi</t>
+  </si>
+  <si>
+    <t>puding</t>
+  </si>
+  <si>
+    <t>temizlik bezi</t>
+  </si>
+  <si>
+    <t>doner</t>
+  </si>
+  <si>
+    <t>tel sehriye</t>
+  </si>
+  <si>
+    <t>bulgur</t>
+  </si>
+  <si>
+    <t>recel</t>
+  </si>
+  <si>
+    <t>armut</t>
+  </si>
+  <si>
+    <t>simit</t>
+  </si>
+  <si>
+    <t>pide</t>
+  </si>
+  <si>
+    <t>karbonat</t>
   </si>
   <si>
     <t>cop poseti</t>
   </si>
   <si>
+    <t>kalem</t>
+  </si>
+  <si>
+    <t>dis macunu</t>
+  </si>
+  <si>
+    <t>buzdolabi poseti</t>
+  </si>
+  <si>
+    <t>bitki cayi</t>
+  </si>
+  <si>
+    <t>oyuncak</t>
+  </si>
+  <si>
     <t>bulyon</t>
   </si>
   <si>
-    <t>serbet</t>
-  </si>
-  <si>
-    <t>misir cerezi</t>
-  </si>
-  <si>
-    <t>tel sehriye</t>
-  </si>
-  <si>
-    <t>tereyag</t>
-  </si>
-  <si>
-    <t>simit</t>
-  </si>
-  <si>
-    <t>pide</t>
-  </si>
-  <si>
-    <t>limonata</t>
-  </si>
-  <si>
-    <t>sandvic</t>
-  </si>
-  <si>
-    <t>meyveli yogurt</t>
-  </si>
-  <si>
-    <t>doner</t>
-  </si>
-  <si>
-    <t>puding</t>
-  </si>
-  <si>
-    <t>tursu</t>
-  </si>
-  <si>
-    <t>bardak</t>
-  </si>
-  <si>
-    <t>labne</t>
-  </si>
-  <si>
-    <t>buzdolabi poseti</t>
+    <t>mercimek</t>
+  </si>
+  <si>
+    <t>sucuk</t>
+  </si>
+  <si>
+    <t>ceviz</t>
+  </si>
+  <si>
+    <t>goz bandi</t>
   </si>
   <si>
     <t>kabartma tozu</t>
   </si>
   <si>
-    <t>temizlik bezi</t>
-  </si>
-  <si>
-    <t>armut</t>
-  </si>
-  <si>
-    <t>yer fistigi</t>
-  </si>
-  <si>
-    <t>recel</t>
-  </si>
-  <si>
-    <t>oyuncak</t>
-  </si>
-  <si>
-    <t>nutella</t>
+    <t>kitap</t>
+  </si>
+  <si>
+    <t>findik</t>
+  </si>
+  <si>
+    <t>corap</t>
+  </si>
+  <si>
+    <t>defter</t>
+  </si>
+  <si>
+    <t>ketcap</t>
+  </si>
+  <si>
+    <t>pisirme kagidi</t>
+  </si>
+  <si>
+    <t>milfoy</t>
+  </si>
+  <si>
+    <t>sarimsak</t>
+  </si>
+  <si>
+    <t>ic giyim</t>
+  </si>
+  <si>
+    <t>kuruyemis</t>
+  </si>
+  <si>
+    <t>jilet</t>
   </si>
   <si>
     <t>mandalina</t>
   </si>
   <si>
-    <t>ceviz</t>
-  </si>
-  <si>
-    <t>goz bandi</t>
-  </si>
-  <si>
-    <t>milfoy</t>
-  </si>
-  <si>
-    <t>pisirme kagidi</t>
-  </si>
-  <si>
-    <t>mercimek</t>
-  </si>
-  <si>
     <t>kolonya</t>
   </si>
   <si>
+    <t>ton baligi</t>
+  </si>
+  <si>
+    <t>gevrek</t>
+  </si>
+  <si>
+    <t>helva</t>
+  </si>
+  <si>
+    <t>fistik</t>
+  </si>
+  <si>
     <t>sunger</t>
   </si>
   <si>
-    <t>nugget</t>
+    <t>vanilin</t>
+  </si>
+  <si>
+    <t>maya</t>
+  </si>
+  <si>
+    <t>bamya</t>
+  </si>
+  <si>
+    <t>bicak</t>
+  </si>
+  <si>
+    <t>kulah</t>
+  </si>
+  <si>
+    <t>kivircik</t>
+  </si>
+  <si>
+    <t>corba</t>
+  </si>
+  <si>
+    <t>bal</t>
+  </si>
+  <si>
+    <t>nohut</t>
+  </si>
+  <si>
+    <t>yag cozucu</t>
+  </si>
+  <si>
+    <t>bulasik kapsulu</t>
+  </si>
+  <si>
+    <t>antep fistigi</t>
+  </si>
+  <si>
+    <t>kakao</t>
+  </si>
+  <si>
+    <t>avokado</t>
+  </si>
+  <si>
+    <t>rus salatasi</t>
+  </si>
+  <si>
+    <t>nane</t>
+  </si>
+  <si>
+    <t>tereyagi</t>
   </si>
   <si>
     <t>pamuk</t>
   </si>
   <si>
-    <t>tereyagi</t>
-  </si>
-  <si>
-    <t>sarimsak</t>
-  </si>
-  <si>
-    <t>ketcap</t>
-  </si>
-  <si>
-    <t>bal</t>
-  </si>
-  <si>
-    <t>sucuk</t>
-  </si>
-  <si>
-    <t>fistik</t>
-  </si>
-  <si>
-    <t>kalem</t>
-  </si>
-  <si>
-    <t>kuruyemis</t>
-  </si>
-  <si>
-    <t>kulah</t>
-  </si>
-  <si>
-    <t>findik</t>
-  </si>
-  <si>
-    <t>mantar</t>
-  </si>
-  <si>
-    <t>cerez</t>
-  </si>
-  <si>
-    <t>ton baligi</t>
-  </si>
-  <si>
-    <t>gevrek</t>
-  </si>
-  <si>
-    <t>rus salatasi</t>
-  </si>
-  <si>
-    <t>sivi sabun</t>
-  </si>
-  <si>
-    <t>yag cozucu</t>
-  </si>
-  <si>
-    <t>nohut</t>
-  </si>
-  <si>
-    <t>jilet</t>
-  </si>
-  <si>
-    <t>vanilin</t>
-  </si>
-  <si>
-    <t>maya</t>
-  </si>
-  <si>
-    <t>corba</t>
-  </si>
-  <si>
-    <t>ic giyim</t>
-  </si>
-  <si>
-    <t>sabun</t>
+    <t>kedi mama</t>
+  </si>
+  <si>
+    <t>link icecek</t>
+  </si>
+  <si>
+    <t>kozlenmis patlican</t>
+  </si>
+  <si>
+    <t>hurma</t>
+  </si>
+  <si>
+    <t>cocuk bezi</t>
+  </si>
+  <si>
+    <t>makine tablet</t>
+  </si>
+  <si>
+    <t>kulak cubugu</t>
+  </si>
+  <si>
+    <t>yuzey temizleyici</t>
+  </si>
+  <si>
+    <t>kadayif</t>
+  </si>
+  <si>
+    <t>tarhana</t>
+  </si>
+  <si>
+    <t>toz deterjan</t>
+  </si>
+  <si>
+    <t>makyaj malzemesi</t>
+  </si>
+  <si>
+    <t>portakal</t>
+  </si>
+  <si>
+    <t>kekik</t>
+  </si>
+  <si>
+    <t>havuc</t>
+  </si>
+  <si>
+    <t>zeytinyagi</t>
+  </si>
+  <si>
+    <t>duzenleyici</t>
+  </si>
+  <si>
+    <t>bulasik teli</t>
+  </si>
+  <si>
+    <t>soslu fistik</t>
+  </si>
+  <si>
+    <t>toka</t>
   </si>
   <si>
     <t>kedi dili</t>
   </si>
   <si>
-    <t>kedi mama</t>
-  </si>
-  <si>
     <t>ayva</t>
   </si>
   <si>
+    <t>sut tozu</t>
+  </si>
+  <si>
+    <t>kagit bardak</t>
+  </si>
+  <si>
+    <t>dus jeli</t>
+  </si>
+  <si>
+    <t>profiterol</t>
+  </si>
+  <si>
+    <t>fume</t>
+  </si>
+  <si>
+    <t>kulaklik</t>
+  </si>
+  <si>
+    <t>kepek ekmek</t>
+  </si>
+  <si>
+    <t>sticker</t>
+  </si>
+  <si>
     <t>toprak</t>
   </si>
   <si>
-    <t>toka</t>
-  </si>
-  <si>
-    <t>kepek ekmek</t>
-  </si>
-  <si>
-    <t>fume</t>
-  </si>
-  <si>
-    <t>bulasik kapsulu</t>
+    <t>lokum</t>
+  </si>
+  <si>
+    <t>havlu</t>
+  </si>
+  <si>
+    <t>zencefil</t>
+  </si>
+  <si>
+    <t>bant</t>
+  </si>
+  <si>
+    <t>kutu</t>
+  </si>
+  <si>
+    <t>iplik</t>
+  </si>
+  <si>
+    <t>yaprak sarma</t>
+  </si>
+  <si>
+    <t>kuru fasulye</t>
   </si>
   <si>
     <t>sac boyasi</t>
   </si>
   <si>
-    <t>yaprak sarma</t>
-  </si>
-  <si>
-    <t>iplik</t>
-  </si>
-  <si>
-    <t>sogan halkasi</t>
-  </si>
-  <si>
-    <t>havlu</t>
-  </si>
-  <si>
-    <t>kekik</t>
-  </si>
-  <si>
-    <t>portakal</t>
-  </si>
-  <si>
     <t>aski</t>
   </si>
   <si>
-    <t>kakao</t>
+    <t>kase</t>
+  </si>
+  <si>
+    <t>mop</t>
+  </si>
+  <si>
+    <t>temizlik sivisi</t>
+  </si>
+  <si>
+    <t>vitamin</t>
+  </si>
+  <si>
+    <t>kurutma topu</t>
+  </si>
+  <si>
+    <t>alez</t>
+  </si>
+  <si>
+    <t>hazir börek</t>
+  </si>
+  <si>
+    <t>yastik kilif</t>
+  </si>
+  <si>
+    <t>tuvalet fircasi</t>
+  </si>
+  <si>
+    <t>cig kofte</t>
+  </si>
+  <si>
+    <t>ampul</t>
+  </si>
+  <si>
+    <t>eriste</t>
+  </si>
+  <si>
+    <t>sandalye</t>
+  </si>
+  <si>
+    <t>kek kabi</t>
+  </si>
+  <si>
+    <t>kutu oyunu</t>
+  </si>
+  <si>
+    <t>yaban mersini</t>
+  </si>
+  <si>
+    <t>cakmak</t>
+  </si>
+  <si>
+    <t>salep</t>
+  </si>
+  <si>
+    <t>parfum</t>
+  </si>
+  <si>
+    <t>dereotu</t>
+  </si>
+  <si>
+    <t>visne</t>
+  </si>
+  <si>
+    <t>ceviz kiracagi</t>
+  </si>
+  <si>
+    <t>silgi</t>
+  </si>
+  <si>
+    <t>fasulye</t>
+  </si>
+  <si>
+    <t>domates sosu</t>
+  </si>
+  <si>
+    <t>pudra seker</t>
+  </si>
+  <si>
+    <t>kayısı</t>
+  </si>
+  <si>
+    <t>kasik</t>
+  </si>
+  <si>
+    <t>findik ezme</t>
+  </si>
+  <si>
+    <t>beyaz sirke</t>
+  </si>
+  <si>
+    <t>uzum</t>
+  </si>
+  <si>
+    <t>sıvı deterjan</t>
+  </si>
+  <si>
+    <t>ispanak</t>
+  </si>
+  <si>
+    <t>bitki</t>
+  </si>
+  <si>
+    <t>greyfurt</t>
+  </si>
+  <si>
+    <t>cicek</t>
+  </si>
+  <si>
+    <t>tac</t>
+  </si>
+  <si>
+    <t>krem</t>
+  </si>
+  <si>
+    <t>boya</t>
+  </si>
+  <si>
+    <t>metre</t>
+  </si>
+  <si>
+    <t>elbise</t>
+  </si>
+  <si>
+    <t>elme</t>
+  </si>
+  <si>
+    <t>elma sirke</t>
+  </si>
+  <si>
+    <t>garnitur</t>
+  </si>
+  <si>
+    <t>maydanoz</t>
+  </si>
+  <si>
+    <t>krem santi</t>
+  </si>
+  <si>
+    <t>tahin</t>
+  </si>
+  <si>
+    <t>temizleme jeli</t>
+  </si>
+  <si>
+    <t>tabak</t>
+  </si>
+  <si>
+    <t>gece lambasi</t>
+  </si>
+  <si>
+    <t>kruvasan</t>
+  </si>
+  <si>
+    <t>ıslak mendil</t>
+  </si>
+  <si>
+    <t>karabiber</t>
+  </si>
+  <si>
+    <t>dolma</t>
+  </si>
+  <si>
+    <t>mikser</t>
+  </si>
+  <si>
+    <t>lavabo kokusu</t>
+  </si>
+  <si>
+    <t>kimyon</t>
+  </si>
+  <si>
+    <t>buzluk</t>
+  </si>
+  <si>
+    <t>cam sil</t>
+  </si>
+  <si>
+    <t>camasir soda</t>
+  </si>
+  <si>
+    <t>el kremi</t>
+  </si>
+  <si>
+    <t>hindistan cevizi</t>
+  </si>
+  <si>
+    <t>krem temizleyici</t>
+  </si>
+  <si>
+    <t>sos</t>
+  </si>
+  <si>
+    <t>dis fircasi</t>
+  </si>
+  <si>
+    <t>tul</t>
+  </si>
+  <si>
+    <t>oralet</t>
+  </si>
+  <si>
+    <t>milkshake</t>
+  </si>
+  <si>
+    <t>oda spreyi</t>
+  </si>
+  <si>
+    <t>canta</t>
+  </si>
+  <si>
+    <t>aseton</t>
+  </si>
+  <si>
+    <t>led isik</t>
+  </si>
+  <si>
+    <t>kori</t>
+  </si>
+  <si>
+    <t>matara</t>
+  </si>
+  <si>
+    <t>oyun hamuru</t>
+  </si>
+  <si>
+    <t>plastik kutu</t>
+  </si>
+  <si>
+    <t>poset cay</t>
+  </si>
+  <si>
+    <t>bone</t>
+  </si>
+  <si>
+    <t>masa lambasi</t>
+  </si>
+  <si>
+    <t>sicak cikolata</t>
+  </si>
+  <si>
+    <t>atlet</t>
+  </si>
+  <si>
+    <t>kremsanti</t>
+  </si>
+  <si>
+    <t>kakolu sut</t>
+  </si>
+  <si>
+    <t>bebek mama</t>
+  </si>
+  <si>
+    <t>kiyma</t>
+  </si>
+  <si>
+    <t>kirec cozucu</t>
+  </si>
+  <si>
+    <t>tost ekmek</t>
+  </si>
+  <si>
+    <t>kako</t>
+  </si>
+  <si>
+    <t>barbunya</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>kuru kayisi</t>
   </si>
   <si>
     <t>kayisi</t>
   </si>
   <si>
-    <t>avokado</t>
-  </si>
-  <si>
-    <t>kitap</t>
-  </si>
-  <si>
-    <t>kuru fasulye</t>
-  </si>
-  <si>
-    <t>corap</t>
-  </si>
-  <si>
-    <t>lokum</t>
-  </si>
-  <si>
-    <t>bulgur</t>
-  </si>
-  <si>
-    <t>profiterol</t>
-  </si>
-  <si>
-    <t>sut tozu</t>
-  </si>
-  <si>
-    <t>kagit bardak</t>
-  </si>
-  <si>
-    <t>link icecek</t>
-  </si>
-  <si>
-    <t>enerji icecegi</t>
-  </si>
-  <si>
-    <t>nane</t>
-  </si>
-  <si>
-    <t>tarhana</t>
-  </si>
-  <si>
-    <t>kadayif</t>
-  </si>
-  <si>
-    <t>hurma</t>
-  </si>
-  <si>
-    <t>bicak</t>
-  </si>
-  <si>
-    <t>toz deterjan</t>
-  </si>
-  <si>
-    <t>makine tablet</t>
-  </si>
-  <si>
-    <t>kivircik</t>
-  </si>
-  <si>
-    <t>bamya</t>
-  </si>
-  <si>
-    <t>cocuk bezi</t>
-  </si>
-  <si>
-    <t>soslu fistik</t>
-  </si>
-  <si>
-    <t>alez</t>
-  </si>
-  <si>
-    <t>kizarmis ekmek</t>
-  </si>
-  <si>
-    <t>bebek mama</t>
-  </si>
-  <si>
-    <t>kirec cozucu</t>
-  </si>
-  <si>
-    <t>kuru kayisi</t>
-  </si>
-  <si>
-    <t>helva</t>
-  </si>
-  <si>
-    <t>ip</t>
-  </si>
-  <si>
-    <t>misir patlagi</t>
-  </si>
-  <si>
     <t>kaju</t>
   </si>
   <si>
+    <t>cevizli sucuk</t>
+  </si>
+  <si>
+    <t>yesil zeytin</t>
+  </si>
+  <si>
+    <t>hazir puding</t>
+  </si>
+  <si>
     <t>rollon</t>
   </si>
   <si>
-    <t>yesil zeytin</t>
-  </si>
-  <si>
-    <t>cevizli sucuk</t>
-  </si>
-  <si>
-    <t>hazir puding</t>
-  </si>
-  <si>
-    <t>bugday ekmegi</t>
-  </si>
-  <si>
     <t>ranch sos</t>
   </si>
   <si>
     <t>kuru uzum</t>
   </si>
   <si>
+    <t>piknik cantasi</t>
+  </si>
+  <si>
     <t>deterjan kutusu</t>
   </si>
   <si>
-    <t>piknik cantasi</t>
-  </si>
-  <si>
     <t>deodorant</t>
   </si>
   <si>
-    <t>hamburger ekmek</t>
-  </si>
-  <si>
-    <t>cilt serum</t>
-  </si>
-  <si>
     <t>strec film</t>
   </si>
   <si>
-    <t>mop</t>
-  </si>
-  <si>
-    <t>hazir borek</t>
-  </si>
-  <si>
-    <t>biber tursu</t>
-  </si>
-  <si>
-    <t>kurutma topu</t>
-  </si>
-  <si>
-    <t>cakmak</t>
-  </si>
-  <si>
-    <t>makyaj malzemesi</t>
-  </si>
-  <si>
-    <t>beyaz sirke</t>
-  </si>
-  <si>
-    <t>findik ezme</t>
-  </si>
-  <si>
-    <t>yuzey temizleyici</t>
-  </si>
-  <si>
-    <t>kasik</t>
-  </si>
-  <si>
-    <t>mikser</t>
-  </si>
-  <si>
-    <t>lavabo kokusu</t>
-  </si>
-  <si>
-    <t>kulak cubugu</t>
-  </si>
-  <si>
-    <t>hazir sandvic</t>
-  </si>
-  <si>
-    <t>pudra seker</t>
-  </si>
-  <si>
-    <t>gece lambasi</t>
-  </si>
-  <si>
-    <t>tahin</t>
-  </si>
-  <si>
-    <t>dolma</t>
-  </si>
-  <si>
-    <t>karabiber</t>
-  </si>
-  <si>
-    <t>ceviz kiracagi</t>
-  </si>
-  <si>
-    <t>silgi</t>
-  </si>
-  <si>
-    <t>dis macunu</t>
-  </si>
-  <si>
-    <t>uzum</t>
-  </si>
-  <si>
-    <t>salep</t>
-  </si>
-  <si>
-    <t>bant</t>
-  </si>
-  <si>
-    <t>kutu</t>
-  </si>
-  <si>
-    <t>kruvasan</t>
-  </si>
-  <si>
-    <t>dus jeli</t>
-  </si>
-  <si>
-    <t>temizleme jeli</t>
-  </si>
-  <si>
-    <t>tabak</t>
-  </si>
-  <si>
-    <t>krem santi</t>
-  </si>
-  <si>
-    <t>elma sirke</t>
-  </si>
-  <si>
-    <t>garnitur</t>
-  </si>
-  <si>
-    <t>fincan</t>
-  </si>
-  <si>
-    <t>maydanoz</t>
-  </si>
-  <si>
-    <t>led isik</t>
-  </si>
-  <si>
-    <t>tul</t>
-  </si>
-  <si>
-    <t>oralet</t>
-  </si>
-  <si>
-    <t>milkshake</t>
-  </si>
-  <si>
-    <t>oda spreyi</t>
-  </si>
-  <si>
-    <t>toz icecek</t>
-  </si>
-  <si>
-    <t>camasir soda</t>
-  </si>
-  <si>
-    <t>kori</t>
-  </si>
-  <si>
-    <t>kimyon</t>
-  </si>
-  <si>
-    <t>bitki cayi</t>
-  </si>
-  <si>
-    <t>canta</t>
-  </si>
-  <si>
-    <t>aseton</t>
-  </si>
-  <si>
-    <t>domates sosu</t>
-  </si>
-  <si>
-    <t>yaban mersini</t>
-  </si>
-  <si>
-    <t>zencefil</t>
-  </si>
-  <si>
-    <t>fasulye</t>
-  </si>
-  <si>
-    <t>sticker</t>
-  </si>
-  <si>
-    <t>plastik kutu</t>
-  </si>
-  <si>
-    <t>oyun hamuru</t>
-  </si>
-  <si>
-    <t>defter</t>
-  </si>
-  <si>
-    <t>matara</t>
-  </si>
-  <si>
-    <t>cilt maskesi</t>
-  </si>
-  <si>
-    <t>barbunya</t>
-  </si>
-  <si>
-    <t>pasta</t>
-  </si>
-  <si>
-    <t>elme</t>
-  </si>
-  <si>
-    <t>el kremi</t>
-  </si>
-  <si>
-    <t>cam sil</t>
-  </si>
-  <si>
-    <t>antep fistigi</t>
-  </si>
-  <si>
-    <t>cay</t>
-  </si>
-  <si>
-    <t>buzluk</t>
-  </si>
-  <si>
-    <t>hindistan cevizi</t>
-  </si>
-  <si>
-    <t>dis fircasi</t>
-  </si>
-  <si>
-    <t>kablolu kulaklik</t>
-  </si>
-  <si>
-    <t>krem temizleyici</t>
-  </si>
-  <si>
-    <t>atlet</t>
-  </si>
-  <si>
-    <t>sos</t>
-  </si>
-  <si>
-    <t>sicak cikolata</t>
-  </si>
-  <si>
-    <t>bone</t>
-  </si>
-  <si>
-    <t>masa lambasi</t>
-  </si>
-  <si>
-    <t>poset cay</t>
-  </si>
-  <si>
-    <t>kagit helva</t>
-  </si>
-  <si>
-    <t>kako</t>
-  </si>
-  <si>
-    <t>tost ekmek</t>
-  </si>
-  <si>
-    <t>kakolu sut</t>
-  </si>
-  <si>
-    <t>kremsanti</t>
-  </si>
-  <si>
-    <t>kiyma</t>
-  </si>
-  <si>
-    <t>vitamin</t>
-  </si>
-  <si>
-    <t>temizlik sivisi</t>
-  </si>
-  <si>
-    <t>tuvalet fircasi</t>
-  </si>
-  <si>
-    <t>yastik kilif</t>
-  </si>
-  <si>
-    <t>kase</t>
-  </si>
-  <si>
-    <t>kutu oyunu</t>
-  </si>
-  <si>
-    <t>kozlenmis patlican</t>
-  </si>
-  <si>
-    <t>kek kabi</t>
-  </si>
-  <si>
-    <t>sandalye</t>
-  </si>
-  <si>
-    <t>eriste</t>
+    <t>mayonez</t>
+  </si>
+  <si>
+    <t>patlican</t>
   </si>
 </sst>
 </file>
@@ -1259,16 +1261,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C286"/>
+  <dimension ref="A1:C291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C286"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1286,10 +1285,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="C2">
-        <v>0.1773584905660377</v>
+        <v>0.16428571428571431</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1297,10 +1296,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C3">
-        <v>0.1169811320754717</v>
+        <v>0.1228571428571429</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1308,10 +1307,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C4">
-        <v>0.11132075471698109</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1319,10 +1318,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C5">
-        <v>0.1056603773584906</v>
+        <v>0.1071428571428571</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1330,10 +1329,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C6">
-        <v>0.10188679245283019</v>
+        <v>0.1014285714285714</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1341,10 +1340,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C7">
-        <v>0.10188679245283019</v>
+        <v>9.8571428571428574E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1352,10 +1351,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C8">
-        <v>9.2452830188679239E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1363,10 +1362,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C9">
-        <v>8.4905660377358486E-2</v>
+        <v>8.8571428571428565E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1374,10 +1373,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C10">
-        <v>8.3018867924528297E-2</v>
+        <v>8.7142857142857147E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1385,10 +1384,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C11">
-        <v>8.3018867924528297E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1396,10 +1395,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C12">
-        <v>7.5471698113207544E-2</v>
+        <v>8.2857142857142851E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1407,10 +1406,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C13">
-        <v>7.3584905660377356E-2</v>
+        <v>7.571428571428572E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1418,10 +1417,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C14">
-        <v>7.3584905660377356E-2</v>
+        <v>7.4285714285714288E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1429,10 +1428,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C15">
-        <v>6.4150943396226415E-2</v>
+        <v>6.4285714285714279E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1440,10 +1439,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C16">
-        <v>6.0377358490566038E-2</v>
+        <v>6.142857142857143E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1451,10 +1450,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C17">
-        <v>5.849056603773585E-2</v>
+        <v>5.8571428571428573E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1462,10 +1461,10 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C18">
-        <v>5.6603773584905662E-2</v>
+        <v>5.5714285714285723E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1473,10 +1472,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C19">
-        <v>5.0943396226415097E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1484,10 +1483,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C20">
-        <v>4.9056603773584909E-2</v>
+        <v>4.7142857142857153E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1495,10 +1494,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>4.716981132075472E-2</v>
+        <v>4.5714285714285707E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1506,10 +1505,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C22">
-        <v>3.7735849056603772E-2</v>
+        <v>4.5714285714285707E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1517,10 +1516,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C23">
-        <v>3.7735849056603772E-2</v>
+        <v>4.2857142857142858E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1528,10 +1527,10 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>3.5849056603773577E-2</v>
+        <v>3.8571428571428569E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1539,10 +1538,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C25">
-        <v>3.3962264150943403E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1550,10 +1549,10 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>3.3962264150943403E-2</v>
+        <v>3.2857142857142863E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1561,10 +1560,10 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>3.3962264150943403E-2</v>
+        <v>3.1428571428571431E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1572,10 +1571,10 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C28">
-        <v>3.2075471698113207E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1583,10 +1582,10 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C29">
-        <v>3.0188679245283019E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1594,10 +1593,10 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C30">
-        <v>3.0188679245283019E-2</v>
+        <v>2.8571428571428571E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1605,10 +1604,10 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C31">
-        <v>3.0188679245283019E-2</v>
+        <v>2.8571428571428571E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1616,10 +1615,10 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C32">
-        <v>3.0188679245283019E-2</v>
+        <v>2.8571428571428571E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1627,10 +1626,10 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C33">
-        <v>3.0188679245283019E-2</v>
+        <v>2.8571428571428571E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1638,10 +1637,10 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>2.8301886792452831E-2</v>
+        <v>2.7142857142857139E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1649,10 +1648,10 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>2.6415094339622639E-2</v>
+        <v>2.7142857142857139E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1660,10 +1659,10 @@
         <v>37</v>
       </c>
       <c r="B36">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C36">
-        <v>2.6415094339622639E-2</v>
+        <v>2.571428571428571E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1671,10 +1670,10 @@
         <v>38</v>
       </c>
       <c r="B37">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C37">
-        <v>2.4528301886792451E-2</v>
+        <v>2.571428571428571E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1682,10 +1681,10 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C38">
-        <v>2.4528301886792451E-2</v>
+        <v>2.571428571428571E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1693,10 +1692,10 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C39">
-        <v>2.4528301886792451E-2</v>
+        <v>2.571428571428571E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1704,10 +1703,10 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C40">
-        <v>2.4528301886792451E-2</v>
+        <v>2.4285714285714289E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1715,10 +1714,10 @@
         <v>42</v>
       </c>
       <c r="B41">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C41">
-        <v>2.0754716981132071E-2</v>
+        <v>2.4285714285714289E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1726,10 +1725,10 @@
         <v>43</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C42">
-        <v>2.0754716981132071E-2</v>
+        <v>2.2857142857142861E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1737,10 +1736,10 @@
         <v>44</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C43">
-        <v>2.0754716981132071E-2</v>
+        <v>2.2857142857142861E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1748,10 +1747,10 @@
         <v>45</v>
       </c>
       <c r="B44">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C44">
-        <v>1.886792452830189E-2</v>
+        <v>2.1428571428571429E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1759,10 +1758,10 @@
         <v>46</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C45">
-        <v>1.886792452830189E-2</v>
+        <v>2.1428571428571429E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1770,10 +1769,10 @@
         <v>47</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C46">
-        <v>1.886792452830189E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1781,10 +1780,10 @@
         <v>48</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C47">
-        <v>1.886792452830189E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1792,10 +1791,10 @@
         <v>49</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C48">
-        <v>1.886792452830189E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1803,10 +1802,10 @@
         <v>50</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>1.886792452830189E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1814,10 +1813,10 @@
         <v>51</v>
       </c>
       <c r="B50">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>1.6981132075471701E-2</v>
+        <v>1.8571428571428569E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1825,10 +1824,10 @@
         <v>52</v>
       </c>
       <c r="B51">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>1.6981132075471701E-2</v>
+        <v>1.8571428571428569E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1836,10 +1835,10 @@
         <v>53</v>
       </c>
       <c r="B52">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C52">
-        <v>1.6981132075471701E-2</v>
+        <v>1.8571428571428569E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1847,10 +1846,10 @@
         <v>54</v>
       </c>
       <c r="B53">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C53">
-        <v>1.6981132075471701E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1858,10 +1857,10 @@
         <v>55</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C54">
-        <v>1.6981132075471701E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1869,10 +1868,10 @@
         <v>56</v>
       </c>
       <c r="B55">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C55">
-        <v>1.6981132075471701E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1880,10 +1879,10 @@
         <v>57</v>
       </c>
       <c r="B56">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C56">
-        <v>1.6981132075471701E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1891,10 +1890,10 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C57">
-        <v>1.6981132075471701E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1902,10 +1901,10 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C58">
-        <v>1.509433962264151E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1913,10 +1912,10 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C59">
-        <v>1.509433962264151E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1924,10 +1923,10 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C60">
-        <v>1.509433962264151E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1935,10 +1934,10 @@
         <v>62</v>
       </c>
       <c r="B61">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C61">
-        <v>1.509433962264151E-2</v>
+        <v>1.5714285714285719E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1946,10 +1945,10 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C62">
-        <v>1.509433962264151E-2</v>
+        <v>1.5714285714285719E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1957,10 +1956,10 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C63">
-        <v>1.320754716981132E-2</v>
+        <v>1.5714285714285719E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1968,10 +1967,10 @@
         <v>65</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C64">
-        <v>1.320754716981132E-2</v>
+        <v>1.5714285714285719E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1979,10 +1978,10 @@
         <v>66</v>
       </c>
       <c r="B65">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C65">
-        <v>1.320754716981132E-2</v>
+        <v>1.5714285714285719E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1990,10 +1989,10 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C66">
-        <v>1.320754716981132E-2</v>
+        <v>1.5714285714285719E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -2001,10 +2000,10 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C67">
-        <v>1.320754716981132E-2</v>
+        <v>1.428571428571429E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -2012,10 +2011,10 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C68">
-        <v>1.320754716981132E-2</v>
+        <v>1.428571428571429E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -2023,10 +2022,10 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>1.320754716981132E-2</v>
+        <v>1.428571428571429E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -2034,10 +2033,10 @@
         <v>71</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C70">
-        <v>1.320754716981132E-2</v>
+        <v>1.285714285714286E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -2045,10 +2044,10 @@
         <v>72</v>
       </c>
       <c r="B71">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>1.320754716981132E-2</v>
+        <v>1.285714285714286E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -2056,10 +2055,10 @@
         <v>73</v>
       </c>
       <c r="B72">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C72">
-        <v>1.132075471698113E-2</v>
+        <v>1.285714285714286E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -2067,10 +2066,10 @@
         <v>74</v>
       </c>
       <c r="B73">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>1.132075471698113E-2</v>
+        <v>1.285714285714286E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -2078,10 +2077,10 @@
         <v>75</v>
       </c>
       <c r="B74">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C74">
-        <v>1.132075471698113E-2</v>
+        <v>1.285714285714286E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -2089,10 +2088,10 @@
         <v>76</v>
       </c>
       <c r="B75">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C75">
-        <v>1.132075471698113E-2</v>
+        <v>1.285714285714286E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -2100,10 +2099,10 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C76">
-        <v>9.433962264150943E-3</v>
+        <v>1.142857142857143E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -2111,10 +2110,10 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C77">
-        <v>9.433962264150943E-3</v>
+        <v>1.142857142857143E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -2122,10 +2121,10 @@
         <v>79</v>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C78">
-        <v>9.433962264150943E-3</v>
+        <v>1.142857142857143E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -2133,10 +2132,10 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C79">
-        <v>9.433962264150943E-3</v>
+        <v>1.142857142857143E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -2144,10 +2143,10 @@
         <v>81</v>
       </c>
       <c r="B80">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C80">
-        <v>9.433962264150943E-3</v>
+        <v>1.142857142857143E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -2155,10 +2154,10 @@
         <v>82</v>
       </c>
       <c r="B81">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C81">
-        <v>9.433962264150943E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -2166,10 +2165,10 @@
         <v>83</v>
       </c>
       <c r="B82">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C82">
-        <v>9.433962264150943E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -2177,10 +2176,10 @@
         <v>84</v>
       </c>
       <c r="B83">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C83">
-        <v>9.433962264150943E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -2188,10 +2187,10 @@
         <v>85</v>
       </c>
       <c r="B84">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C84">
-        <v>9.433962264150943E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -2199,10 +2198,10 @@
         <v>86</v>
       </c>
       <c r="B85">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>9.433962264150943E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -2210,10 +2209,10 @@
         <v>87</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C86">
-        <v>9.433962264150943E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -2221,10 +2220,10 @@
         <v>88</v>
       </c>
       <c r="B87">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>9.433962264150943E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -2232,10 +2231,10 @@
         <v>89</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C88">
-        <v>9.433962264150943E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -2243,10 +2242,10 @@
         <v>90</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C89">
-        <v>9.433962264150943E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -2254,10 +2253,10 @@
         <v>91</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>9.433962264150943E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -2265,10 +2264,10 @@
         <v>92</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>9.433962264150943E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -2276,10 +2275,10 @@
         <v>93</v>
       </c>
       <c r="B92">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C92">
-        <v>7.5471698113207548E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -2287,10 +2286,10 @@
         <v>94</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C93">
-        <v>7.5471698113207548E-3</v>
+        <v>8.5714285714285719E-3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -2298,10 +2297,10 @@
         <v>95</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C94">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -2309,10 +2308,10 @@
         <v>96</v>
       </c>
       <c r="B95">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C95">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -2320,10 +2319,10 @@
         <v>97</v>
       </c>
       <c r="B96">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C96">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -2331,10 +2330,10 @@
         <v>98</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C97">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -2342,10 +2341,10 @@
         <v>99</v>
       </c>
       <c r="B98">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C98">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -2353,10 +2352,10 @@
         <v>100</v>
       </c>
       <c r="B99">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C99">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -2364,10 +2363,10 @@
         <v>101</v>
       </c>
       <c r="B100">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C100">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -2375,10 +2374,10 @@
         <v>102</v>
       </c>
       <c r="B101">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C101">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -2386,10 +2385,10 @@
         <v>103</v>
       </c>
       <c r="B102">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C102">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -2397,10 +2396,10 @@
         <v>104</v>
       </c>
       <c r="B103">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C103">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -2408,10 +2407,10 @@
         <v>105</v>
       </c>
       <c r="B104">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C104">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -2419,10 +2418,10 @@
         <v>106</v>
       </c>
       <c r="B105">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C105">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -2430,10 +2429,10 @@
         <v>107</v>
       </c>
       <c r="B106">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C106">
-        <v>7.5471698113207548E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -2441,10 +2440,10 @@
         <v>108</v>
       </c>
       <c r="B107">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C107">
-        <v>5.6603773584905656E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -2452,10 +2451,10 @@
         <v>109</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C108">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -2463,10 +2462,10 @@
         <v>110</v>
       </c>
       <c r="B109">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C109">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -2474,10 +2473,10 @@
         <v>111</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C110">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -2485,10 +2484,10 @@
         <v>112</v>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C111">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -2496,10 +2495,10 @@
         <v>113</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C112">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -2507,10 +2506,10 @@
         <v>114</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C113">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -2518,10 +2517,10 @@
         <v>115</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C114">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -2529,10 +2528,10 @@
         <v>116</v>
       </c>
       <c r="B115">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C115">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -2540,10 +2539,10 @@
         <v>117</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -2551,10 +2550,10 @@
         <v>118</v>
       </c>
       <c r="B117">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C117">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -2562,10 +2561,10 @@
         <v>119</v>
       </c>
       <c r="B118">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C118">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -2573,10 +2572,10 @@
         <v>120</v>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C119">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -2584,10 +2583,10 @@
         <v>121</v>
       </c>
       <c r="B120">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C120">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -2595,10 +2594,10 @@
         <v>122</v>
       </c>
       <c r="B121">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C121">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -2606,10 +2605,10 @@
         <v>123</v>
       </c>
       <c r="B122">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C122">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -2617,10 +2616,10 @@
         <v>124</v>
       </c>
       <c r="B123">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C123">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -2628,10 +2627,10 @@
         <v>125</v>
       </c>
       <c r="B124">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C124">
-        <v>5.6603773584905656E-3</v>
+        <v>5.7142857142857143E-3</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -2642,7 +2641,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -2653,7 +2652,7 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -2664,7 +2663,7 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -2675,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -2686,7 +2685,7 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -2697,7 +2696,7 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -2708,7 +2707,7 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -2719,7 +2718,7 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>5.6603773584905656E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -2727,10 +2726,10 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C133">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -2738,10 +2737,10 @@
         <v>135</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C134">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -2749,10 +2748,10 @@
         <v>136</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C135">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -2760,10 +2759,10 @@
         <v>137</v>
       </c>
       <c r="B136">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C136">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -2771,10 +2770,10 @@
         <v>138</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C137">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -2782,10 +2781,10 @@
         <v>139</v>
       </c>
       <c r="B138">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C138">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -2793,10 +2792,10 @@
         <v>140</v>
       </c>
       <c r="B139">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -2804,10 +2803,10 @@
         <v>141</v>
       </c>
       <c r="B140">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C140">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -2815,10 +2814,10 @@
         <v>142</v>
       </c>
       <c r="B141">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C141">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -2826,10 +2825,10 @@
         <v>143</v>
       </c>
       <c r="B142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C142">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -2837,10 +2836,10 @@
         <v>144</v>
       </c>
       <c r="B143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C143">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -2848,10 +2847,10 @@
         <v>145</v>
       </c>
       <c r="B144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C144">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -2859,10 +2858,10 @@
         <v>146</v>
       </c>
       <c r="B145">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C145">
-        <v>3.773584905660377E-3</v>
+        <v>4.2857142857142859E-3</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -2873,7 +2872,7 @@
         <v>2</v>
       </c>
       <c r="C146">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -2884,7 +2883,7 @@
         <v>2</v>
       </c>
       <c r="C147">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -2895,7 +2894,7 @@
         <v>2</v>
       </c>
       <c r="C148">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -2906,7 +2905,7 @@
         <v>2</v>
       </c>
       <c r="C149">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -2917,7 +2916,7 @@
         <v>2</v>
       </c>
       <c r="C150">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -2928,7 +2927,7 @@
         <v>2</v>
       </c>
       <c r="C151">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -2939,7 +2938,7 @@
         <v>2</v>
       </c>
       <c r="C152">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -2950,7 +2949,7 @@
         <v>2</v>
       </c>
       <c r="C153">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -2961,7 +2960,7 @@
         <v>2</v>
       </c>
       <c r="C154">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -2972,7 +2971,7 @@
         <v>2</v>
       </c>
       <c r="C155">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -2983,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="C156">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -2994,7 +2993,7 @@
         <v>2</v>
       </c>
       <c r="C157">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -3005,7 +3004,7 @@
         <v>2</v>
       </c>
       <c r="C158">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
@@ -3016,7 +3015,7 @@
         <v>2</v>
       </c>
       <c r="C159">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -3027,7 +3026,7 @@
         <v>2</v>
       </c>
       <c r="C160">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -3038,7 +3037,7 @@
         <v>2</v>
       </c>
       <c r="C161">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -3049,7 +3048,7 @@
         <v>2</v>
       </c>
       <c r="C162">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -3060,7 +3059,7 @@
         <v>2</v>
       </c>
       <c r="C163">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -3071,7 +3070,7 @@
         <v>2</v>
       </c>
       <c r="C164">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -3082,7 +3081,7 @@
         <v>2</v>
       </c>
       <c r="C165">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -3093,7 +3092,7 @@
         <v>2</v>
       </c>
       <c r="C166">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -3104,7 +3103,7 @@
         <v>2</v>
       </c>
       <c r="C167">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -3115,7 +3114,7 @@
         <v>2</v>
       </c>
       <c r="C168">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -3126,7 +3125,7 @@
         <v>2</v>
       </c>
       <c r="C169">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -3137,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="C170">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -3148,7 +3147,7 @@
         <v>2</v>
       </c>
       <c r="C171">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -3159,7 +3158,7 @@
         <v>2</v>
       </c>
       <c r="C172">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -3170,7 +3169,7 @@
         <v>2</v>
       </c>
       <c r="C173">
-        <v>3.773584905660377E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -3178,10 +3177,10 @@
         <v>175</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C174">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -3189,10 +3188,10 @@
         <v>176</v>
       </c>
       <c r="B175">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C175">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -3200,10 +3199,10 @@
         <v>177</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C176">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -3211,10 +3210,10 @@
         <v>178</v>
       </c>
       <c r="B177">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C177">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -3222,10 +3221,10 @@
         <v>179</v>
       </c>
       <c r="B178">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C178">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -3233,10 +3232,10 @@
         <v>180</v>
       </c>
       <c r="B179">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C179">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -3244,10 +3243,10 @@
         <v>181</v>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C180">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -3255,10 +3254,10 @@
         <v>182</v>
       </c>
       <c r="B181">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C181">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -3266,10 +3265,10 @@
         <v>183</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C182">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -3277,10 +3276,10 @@
         <v>184</v>
       </c>
       <c r="B183">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C183">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -3288,10 +3287,10 @@
         <v>185</v>
       </c>
       <c r="B184">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C184">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
@@ -3299,10 +3298,10 @@
         <v>186</v>
       </c>
       <c r="B185">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C185">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -3310,10 +3309,10 @@
         <v>187</v>
       </c>
       <c r="B186">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C186">
-        <v>1.8867924528301889E-3</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -3324,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="C187">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -3335,7 +3334,7 @@
         <v>1</v>
       </c>
       <c r="C188">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
@@ -3346,7 +3345,7 @@
         <v>1</v>
       </c>
       <c r="C189">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -3357,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="C190">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -3368,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="C191">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -3379,7 +3378,7 @@
         <v>1</v>
       </c>
       <c r="C192">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -3390,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="C193">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -3401,7 +3400,7 @@
         <v>1</v>
       </c>
       <c r="C194">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
@@ -3412,7 +3411,7 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -3423,7 +3422,7 @@
         <v>1</v>
       </c>
       <c r="C196">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -3434,7 +3433,7 @@
         <v>1</v>
       </c>
       <c r="C197">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -3445,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="C198">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -3456,7 +3455,7 @@
         <v>1</v>
       </c>
       <c r="C199">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -3467,7 +3466,7 @@
         <v>1</v>
       </c>
       <c r="C200">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -3478,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="C201">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -3489,7 +3488,7 @@
         <v>1</v>
       </c>
       <c r="C202">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
@@ -3500,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="C203">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
@@ -3511,7 +3510,7 @@
         <v>1</v>
       </c>
       <c r="C204">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
@@ -3522,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="C205">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
@@ -3533,7 +3532,7 @@
         <v>1</v>
       </c>
       <c r="C206">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
@@ -3544,7 +3543,7 @@
         <v>1</v>
       </c>
       <c r="C207">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -3555,7 +3554,7 @@
         <v>1</v>
       </c>
       <c r="C208">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
@@ -3566,7 +3565,7 @@
         <v>1</v>
       </c>
       <c r="C209">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
@@ -3577,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="C210">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -3588,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="C211">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -3599,7 +3598,7 @@
         <v>1</v>
       </c>
       <c r="C212">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -3610,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="C213">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
@@ -3621,7 +3620,7 @@
         <v>1</v>
       </c>
       <c r="C214">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -3632,7 +3631,7 @@
         <v>1</v>
       </c>
       <c r="C215">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
@@ -3643,7 +3642,7 @@
         <v>1</v>
       </c>
       <c r="C216">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
@@ -3654,7 +3653,7 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
@@ -3665,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="C218">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
@@ -3676,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="C219">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
@@ -3687,7 +3686,7 @@
         <v>1</v>
       </c>
       <c r="C220">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
@@ -3698,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="C221">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
@@ -3709,7 +3708,7 @@
         <v>1</v>
       </c>
       <c r="C222">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
@@ -3720,7 +3719,7 @@
         <v>1</v>
       </c>
       <c r="C223">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
@@ -3731,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="C224">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
@@ -3742,7 +3741,7 @@
         <v>1</v>
       </c>
       <c r="C225">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
@@ -3753,7 +3752,7 @@
         <v>1</v>
       </c>
       <c r="C226">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
@@ -3764,7 +3763,7 @@
         <v>1</v>
       </c>
       <c r="C227">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
@@ -3775,7 +3774,7 @@
         <v>1</v>
       </c>
       <c r="C228">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
@@ -3786,7 +3785,7 @@
         <v>1</v>
       </c>
       <c r="C229">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
@@ -3797,7 +3796,7 @@
         <v>1</v>
       </c>
       <c r="C230">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
@@ -3808,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="C231">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
@@ -3819,7 +3818,7 @@
         <v>1</v>
       </c>
       <c r="C232">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
@@ -3830,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="C233">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
@@ -3841,7 +3840,7 @@
         <v>1</v>
       </c>
       <c r="C234">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
@@ -3852,7 +3851,7 @@
         <v>1</v>
       </c>
       <c r="C235">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
@@ -3863,7 +3862,7 @@
         <v>1</v>
       </c>
       <c r="C236">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
@@ -3874,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="C237">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
@@ -3885,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="C238">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
@@ -3896,7 +3895,7 @@
         <v>1</v>
       </c>
       <c r="C239">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
@@ -3907,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="C240">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
@@ -3918,7 +3917,7 @@
         <v>1</v>
       </c>
       <c r="C241">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
@@ -3929,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="C242">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
@@ -3940,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="C243">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
@@ -3951,7 +3950,7 @@
         <v>1</v>
       </c>
       <c r="C244">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
@@ -3962,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="C245">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
@@ -3973,7 +3972,7 @@
         <v>1</v>
       </c>
       <c r="C246">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
@@ -3984,7 +3983,7 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
@@ -3995,7 +3994,7 @@
         <v>1</v>
       </c>
       <c r="C248">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
@@ -4006,7 +4005,7 @@
         <v>1</v>
       </c>
       <c r="C249">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
@@ -4017,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="C250">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
@@ -4028,7 +4027,7 @@
         <v>1</v>
       </c>
       <c r="C251">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
@@ -4039,7 +4038,7 @@
         <v>1</v>
       </c>
       <c r="C252">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
@@ -4050,7 +4049,7 @@
         <v>1</v>
       </c>
       <c r="C253">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
@@ -4061,7 +4060,7 @@
         <v>1</v>
       </c>
       <c r="C254">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
@@ -4072,7 +4071,7 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
@@ -4083,7 +4082,7 @@
         <v>1</v>
       </c>
       <c r="C256">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
@@ -4094,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="C257">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
@@ -4105,7 +4104,7 @@
         <v>1</v>
       </c>
       <c r="C258">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
@@ -4116,7 +4115,7 @@
         <v>1</v>
       </c>
       <c r="C259">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
@@ -4127,7 +4126,7 @@
         <v>1</v>
       </c>
       <c r="C260">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
@@ -4138,7 +4137,7 @@
         <v>1</v>
       </c>
       <c r="C261">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
@@ -4149,7 +4148,7 @@
         <v>1</v>
       </c>
       <c r="C262">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
@@ -4160,7 +4159,7 @@
         <v>1</v>
       </c>
       <c r="C263">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
@@ -4171,7 +4170,7 @@
         <v>1</v>
       </c>
       <c r="C264">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
@@ -4182,7 +4181,7 @@
         <v>1</v>
       </c>
       <c r="C265">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
@@ -4193,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="C266">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
@@ -4204,7 +4203,7 @@
         <v>1</v>
       </c>
       <c r="C267">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
@@ -4215,7 +4214,7 @@
         <v>1</v>
       </c>
       <c r="C268">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
@@ -4226,7 +4225,7 @@
         <v>1</v>
       </c>
       <c r="C269">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
@@ -4237,7 +4236,7 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
@@ -4248,7 +4247,7 @@
         <v>1</v>
       </c>
       <c r="C271">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
@@ -4259,7 +4258,7 @@
         <v>1</v>
       </c>
       <c r="C272">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
@@ -4270,7 +4269,7 @@
         <v>1</v>
       </c>
       <c r="C273">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
@@ -4281,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
@@ -4292,7 +4291,7 @@
         <v>1</v>
       </c>
       <c r="C275">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
@@ -4303,7 +4302,7 @@
         <v>1</v>
       </c>
       <c r="C276">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
@@ -4314,7 +4313,7 @@
         <v>1</v>
       </c>
       <c r="C277">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
@@ -4325,7 +4324,7 @@
         <v>1</v>
       </c>
       <c r="C278">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
@@ -4336,7 +4335,7 @@
         <v>1</v>
       </c>
       <c r="C279">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
@@ -4347,7 +4346,7 @@
         <v>1</v>
       </c>
       <c r="C280">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
@@ -4358,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="C281">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
@@ -4369,7 +4368,7 @@
         <v>1</v>
       </c>
       <c r="C282">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
@@ -4380,7 +4379,7 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
@@ -4391,7 +4390,7 @@
         <v>1</v>
       </c>
       <c r="C284">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
@@ -4402,7 +4401,7 @@
         <v>1</v>
       </c>
       <c r="C285">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
@@ -4413,7 +4412,62 @@
         <v>1</v>
       </c>
       <c r="C286">
-        <v>1.8867924528301889E-3</v>
+        <v>1.428571428571429E-3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>288</v>
+      </c>
+      <c r="B287">
+        <v>1</v>
+      </c>
+      <c r="C287">
+        <v>1.428571428571429E-3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>289</v>
+      </c>
+      <c r="B288">
+        <v>1</v>
+      </c>
+      <c r="C288">
+        <v>1.428571428571429E-3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>290</v>
+      </c>
+      <c r="B289">
+        <v>1</v>
+      </c>
+      <c r="C289">
+        <v>1.428571428571429E-3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>291</v>
+      </c>
+      <c r="B290">
+        <v>1</v>
+      </c>
+      <c r="C290">
+        <v>1.428571428571429E-3</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>292</v>
+      </c>
+      <c r="B291">
+        <v>1</v>
+      </c>
+      <c r="C291">
+        <v>1.428571428571429E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>